<commit_message>
Feature / Adição dos dicionários atualizados e atualização na documentação docx
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionarioFuncionarios.xlsx
+++ b/dicionario_dados/dicionarioFuncionarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alunosatcedu-my.sharepoint.com/personal/rhyan_7423_alunosatc_edu_br/Documents/Engenharia de Computação/Banco de Dados II/Trabalho Final/Dicionários das tabelas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{7B3A1A37-D8C2-4C3E-A4E2-42D07B7A357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FB21632-E8F8-467B-91D0-3B7513ECBD0B}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{7B3A1A37-D8C2-4C3E-A4E2-42D07B7A357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46218CDF-25EC-4575-94BF-AC24784A90C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Tabela</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Nome do índice</t>
   </si>
   <si>
-    <t>funcionario_id</t>
-  </si>
-  <si>
-    <t>funcionarios</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os funcionários cadastrados</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>cargo</t>
   </si>
   <si>
-    <t>varchar(30)</t>
-  </si>
-  <si>
     <t>varchar(40)</t>
   </si>
   <si>
@@ -137,9 +128,6 @@
     <t>0 – 40</t>
   </si>
   <si>
-    <t>0 – 30</t>
-  </si>
-  <si>
     <t>CPF do funcionário</t>
   </si>
   <si>
@@ -155,10 +143,58 @@
     <t>Nome do funcionário</t>
   </si>
   <si>
-    <t>varchar(70)</t>
-  </si>
-  <si>
-    <t>1 – 70</t>
+    <t>Funcionarios</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>1 – 100</t>
+  </si>
+  <si>
+    <t>varchar(14)</t>
+  </si>
+  <si>
+    <t>0 – 14</t>
+  </si>
+  <si>
+    <t>ativo</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>0 – 1</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>0 – 50</t>
+  </si>
+  <si>
+    <t>permissao_id</t>
+  </si>
+  <si>
+    <t>1 - sem limite</t>
+  </si>
+  <si>
+    <t>Foreign Key da tabela de permissões correspondente a permissão do usuário no sistema</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Identificação se o funcionário está habilitado ou desabilitado</t>
+  </si>
+  <si>
+    <t>PRIMARY</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
 </sst>
 </file>
@@ -281,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -295,6 +331,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -312,18 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,64 +685,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F16" sqref="F16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="3.88671875" customWidth="1"/>
     <col min="7" max="7" width="3.6640625" customWidth="1"/>
-    <col min="8" max="8" width="67.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -721,10 +763,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="13"/>
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -739,189 +781,243 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="13"/>
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="13"/>
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="13"/>
+      <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="13"/>
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="6"/>
+      <c r="A15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
+  <mergeCells count="23">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -929,19 +1025,12 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:H13"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
[Fix] Alternado Relatório para estado anterior, adicionando scipts atualizados
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionarioFuncionarios.xlsx
+++ b/dicionario_dados/dicionarioFuncionarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alunosatcedu-my.sharepoint.com/personal/rhyan_7423_alunosatc_edu_br/Documents/Engenharia de Computação/Banco de Dados II/Trabalho Final/Dicionários das tabelas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{7B3A1A37-D8C2-4C3E-A4E2-42D07B7A357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FB21632-E8F8-467B-91D0-3B7513ECBD0B}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{7B3A1A37-D8C2-4C3E-A4E2-42D07B7A357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46218CDF-25EC-4575-94BF-AC24784A90C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Tabela</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Nome do índice</t>
   </si>
   <si>
-    <t>funcionario_id</t>
-  </si>
-  <si>
-    <t>funcionarios</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os funcionários cadastrados</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>cargo</t>
   </si>
   <si>
-    <t>varchar(30)</t>
-  </si>
-  <si>
     <t>varchar(40)</t>
   </si>
   <si>
@@ -137,9 +128,6 @@
     <t>0 – 40</t>
   </si>
   <si>
-    <t>0 – 30</t>
-  </si>
-  <si>
     <t>CPF do funcionário</t>
   </si>
   <si>
@@ -155,10 +143,58 @@
     <t>Nome do funcionário</t>
   </si>
   <si>
-    <t>varchar(70)</t>
-  </si>
-  <si>
-    <t>1 – 70</t>
+    <t>Funcionarios</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>1 – 100</t>
+  </si>
+  <si>
+    <t>varchar(14)</t>
+  </si>
+  <si>
+    <t>0 – 14</t>
+  </si>
+  <si>
+    <t>ativo</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>0 – 1</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>0 – 50</t>
+  </si>
+  <si>
+    <t>permissao_id</t>
+  </si>
+  <si>
+    <t>1 - sem limite</t>
+  </si>
+  <si>
+    <t>Foreign Key da tabela de permissões correspondente a permissão do usuário no sistema</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Identificação se o funcionário está habilitado ou desabilitado</t>
+  </si>
+  <si>
+    <t>PRIMARY</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
 </sst>
 </file>
@@ -281,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -295,6 +331,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -312,18 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,64 +685,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F16" sqref="F16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="3.88671875" customWidth="1"/>
     <col min="7" max="7" width="3.6640625" customWidth="1"/>
-    <col min="8" max="8" width="67.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -721,10 +763,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="13"/>
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -739,189 +781,243 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="13"/>
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="13"/>
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="13"/>
+      <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="13"/>
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="6"/>
+      <c r="A15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
+  <mergeCells count="23">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -929,19 +1025,12 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:H13"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>